<commit_message>
[Chore] Install read-excel-file module
</commit_message>
<xml_diff>
--- a/server/src/restinfos.xlsx
+++ b/server/src/restinfos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeomhyeji/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeomhyeji/Desktop/projects/MIJIworld/server/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B11EFE1-772B-114F-8255-60C367F2E8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1524D09-FB58-F244-BCAD-5144CFC15186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{21BFD20C-F461-4008-810F-8834C880AE86}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{21BFD20C-F461-4008-810F-8834C880AE86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="577">
   <si>
     <t>#0463D2</t>
   </si>
@@ -2999,69 +2999,78 @@
     <t>https://place.map.kakao.com/18778526</t>
   </si>
   <si>
+    <t>https://place.map.kakao.com/539411343</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/16989098</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/26603579</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/586935295</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/16034968</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/523907573</t>
+  </si>
+  <si>
+    <t>https://map.naver.com/v5/entry/place/245978217?c=14135991.5772182,4517324.1576999,19,0,0,0,dh</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/21130631</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/20950913</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/8710354</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/931679409</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/17672246</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/10371912</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/7908378</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/17357597</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/25462155</t>
+  </si>
+  <si>
+    <t>https://map.naver.com/v5/entry/place/1735679364?c=14143167.4097060,4542617.0198217,19,0,0,0,dh</t>
+  </si>
+  <si>
+    <t>https://place.map.kakao.com/23642006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kakaoReviewUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://map.naver.com/v5/entry/place/34907751?c=14133888.3846828,4519968.3825312,15,0,0,0,dh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pintop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pinleft</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>https://place.map.kakao.com/1675286779</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/539411343</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/16989098</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/26603579</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/586935295</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/16034968</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/523907573</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/245978217?c=14135991.5772182,4517324.1576999,19,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/21130631</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/20950913</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/8710354</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/931679409</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/17672246</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/10371912</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/7908378</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/17357597</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/25462155</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/1735679364?c=14143167.4097060,4542617.0198217,19,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://place.map.kakao.com/23642006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kakaoReviewUrl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/34907751?c=14133888.3846828,4519968.3825312,15,0,0,0,dh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3261,7 +3270,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3296,9 +3305,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -3619,18 +3625,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41FF5E1-E7C0-4FE7-B208-B8C1E78BE041}">
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="131" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView tabSelected="1" topLeftCell="AC9" zoomScale="131" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
-  <cols>
-    <col min="34" max="34" width="8.83203125" style="12"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3728,13 +3731,19 @@
         <v>32</v>
       </c>
       <c r="AG1" t="s">
-        <v>573</v>
-      </c>
-      <c r="AI1" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
+      <c r="AJ1" t="s">
+        <v>574</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>575</v>
+      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:37">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3832,13 +3841,19 @@
         <v>67</v>
       </c>
       <c r="AG2" s="11" t="s">
-        <v>572</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>574</v>
+        <v>571</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="AJ2">
+        <v>45</v>
+      </c>
+      <c r="AK2">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:37">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3938,11 +3953,17 @@
       <c r="AG3" t="s">
         <v>546</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AH3" t="s">
         <v>525</v>
       </c>
+      <c r="AJ3">
+        <v>82</v>
+      </c>
+      <c r="AK3">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" ht="48">
+    <row r="4" spans="1:37" ht="48">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4036,11 +4057,17 @@
       <c r="AG4" t="s">
         <v>547</v>
       </c>
-      <c r="AH4" s="12" t="s">
+      <c r="AH4" t="s">
         <v>524</v>
       </c>
+      <c r="AJ4">
+        <v>60</v>
+      </c>
+      <c r="AK4">
+        <v>14.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:35" ht="32">
+    <row r="5" spans="1:37" ht="32">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4140,11 +4167,17 @@
       <c r="AG5" t="s">
         <v>548</v>
       </c>
-      <c r="AH5" s="12" t="s">
+      <c r="AH5" t="s">
         <v>526</v>
       </c>
+      <c r="AJ5">
+        <v>59</v>
+      </c>
+      <c r="AK5">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:35" ht="48">
+    <row r="6" spans="1:37" ht="48">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4244,11 +4277,17 @@
       <c r="AG6" t="s">
         <v>549</v>
       </c>
-      <c r="AH6" s="12" t="s">
+      <c r="AH6" t="s">
         <v>527</v>
       </c>
+      <c r="AJ6">
+        <v>56</v>
+      </c>
+      <c r="AK6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:37">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4348,11 +4387,17 @@
       <c r="AG7" t="s">
         <v>550</v>
       </c>
-      <c r="AH7" s="12" t="s">
+      <c r="AH7" t="s">
         <v>528</v>
       </c>
+      <c r="AJ7">
+        <v>47</v>
+      </c>
+      <c r="AK7">
+        <v>13</v>
+      </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:37">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4452,11 +4497,17 @@
       <c r="AG8" t="s">
         <v>551</v>
       </c>
-      <c r="AH8" s="12" t="s">
+      <c r="AH8" t="s">
         <v>529</v>
       </c>
+      <c r="AJ8">
+        <v>51</v>
+      </c>
+      <c r="AK8">
+        <v>21.5</v>
+      </c>
     </row>
-    <row r="9" spans="1:35" ht="48">
+    <row r="9" spans="1:37" ht="48">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4556,11 +4607,17 @@
       <c r="AG9" t="s">
         <v>552</v>
       </c>
-      <c r="AH9" s="12" t="s">
+      <c r="AH9" t="s">
         <v>530</v>
       </c>
+      <c r="AJ9">
+        <v>66</v>
+      </c>
+      <c r="AK9">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:35" ht="48">
+    <row r="10" spans="1:37" ht="48">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4660,11 +4717,17 @@
       <c r="AG10" t="s">
         <v>553</v>
       </c>
-      <c r="AH10" s="12" t="s">
+      <c r="AH10" t="s">
         <v>532</v>
       </c>
+      <c r="AJ10">
+        <v>61</v>
+      </c>
+      <c r="AK10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:37">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4737,14 +4800,20 @@
       <c r="AF11">
         <v>102</v>
       </c>
-      <c r="AG11" t="s">
-        <v>554</v>
-      </c>
-      <c r="AH11" s="12" t="s">
+      <c r="AG11" s="11" t="s">
+        <v>576</v>
+      </c>
+      <c r="AH11" t="s">
         <v>531</v>
       </c>
+      <c r="AJ11">
+        <v>66</v>
+      </c>
+      <c r="AK11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:37">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4842,13 +4911,19 @@
         <v>187</v>
       </c>
       <c r="AG12" t="s">
-        <v>555</v>
-      </c>
-      <c r="AH12" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="AH12" t="s">
         <v>533</v>
       </c>
+      <c r="AJ12">
+        <v>55</v>
+      </c>
+      <c r="AK12">
+        <v>40</v>
+      </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:37">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4946,13 +5021,19 @@
         <v>542</v>
       </c>
       <c r="AG13" t="s">
-        <v>556</v>
-      </c>
-      <c r="AH13" s="12" t="s">
+        <v>555</v>
+      </c>
+      <c r="AH13" t="s">
         <v>534</v>
       </c>
+      <c r="AJ13">
+        <v>38</v>
+      </c>
+      <c r="AK13">
+        <v>30</v>
+      </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:37">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5050,13 +5131,19 @@
         <v>492</v>
       </c>
       <c r="AG14" t="s">
-        <v>557</v>
-      </c>
-      <c r="AH14" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="AH14" t="s">
         <v>535</v>
       </c>
+      <c r="AJ14">
+        <v>61</v>
+      </c>
+      <c r="AK14">
+        <v>34.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:35" ht="18">
+    <row r="15" spans="1:37" ht="18">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5139,13 +5226,19 @@
         <v>1</v>
       </c>
       <c r="AG15" t="s">
-        <v>558</v>
-      </c>
-      <c r="AH15" s="12" t="s">
-        <v>571</v>
+        <v>557</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>570</v>
+      </c>
+      <c r="AJ15">
+        <v>59</v>
+      </c>
+      <c r="AK15">
+        <v>40.5</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:37">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5243,13 +5336,19 @@
         <v>289</v>
       </c>
       <c r="AG16" t="s">
-        <v>559</v>
-      </c>
-      <c r="AH16" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="AH16" t="s">
         <v>536</v>
       </c>
+      <c r="AJ16">
+        <v>37</v>
+      </c>
+      <c r="AK16">
+        <v>39</v>
+      </c>
     </row>
-    <row r="17" spans="1:34">
+    <row r="17" spans="1:37">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5347,13 +5446,19 @@
         <v>995</v>
       </c>
       <c r="AG17" t="s">
+        <v>559</v>
+      </c>
+      <c r="AH17" t="s">
         <v>560</v>
       </c>
-      <c r="AH17" s="12" t="s">
-        <v>561</v>
+      <c r="AJ17">
+        <v>65</v>
+      </c>
+      <c r="AK17">
+        <v>42.5</v>
       </c>
     </row>
-    <row r="18" spans="1:34">
+    <row r="18" spans="1:37">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5451,13 +5556,19 @@
         <v>53</v>
       </c>
       <c r="AG18" t="s">
-        <v>562</v>
-      </c>
-      <c r="AH18" s="12" t="s">
+        <v>561</v>
+      </c>
+      <c r="AH18" t="s">
         <v>537</v>
       </c>
+      <c r="AJ18">
+        <v>49</v>
+      </c>
+      <c r="AK18">
+        <v>31</v>
+      </c>
     </row>
-    <row r="19" spans="1:34">
+    <row r="19" spans="1:37">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5555,13 +5666,19 @@
         <v>1116</v>
       </c>
       <c r="AG19" t="s">
-        <v>563</v>
-      </c>
-      <c r="AH19" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="AH19" t="s">
         <v>538</v>
       </c>
+      <c r="AJ19">
+        <v>48</v>
+      </c>
+      <c r="AK19">
+        <v>24</v>
+      </c>
     </row>
-    <row r="20" spans="1:34" ht="42">
+    <row r="20" spans="1:37" ht="64">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5659,13 +5776,19 @@
         <v>136</v>
       </c>
       <c r="AG20" t="s">
-        <v>564</v>
-      </c>
-      <c r="AH20" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="AH20" t="s">
         <v>539</v>
       </c>
+      <c r="AJ20">
+        <v>43</v>
+      </c>
+      <c r="AK20">
+        <v>20</v>
+      </c>
     </row>
-    <row r="21" spans="1:34" ht="48">
+    <row r="21" spans="1:37" ht="48">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5763,13 +5886,19 @@
         <v>454</v>
       </c>
       <c r="AG21" t="s">
-        <v>565</v>
-      </c>
-      <c r="AH21" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="AH21" t="s">
         <v>540</v>
       </c>
+      <c r="AJ21">
+        <v>43</v>
+      </c>
+      <c r="AK21">
+        <v>72</v>
+      </c>
     </row>
-    <row r="22" spans="1:34" ht="32">
+    <row r="22" spans="1:37" ht="32">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5867,13 +5996,19 @@
         <v>164</v>
       </c>
       <c r="AG22" t="s">
-        <v>566</v>
-      </c>
-      <c r="AH22" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="AH22" t="s">
         <v>541</v>
       </c>
+      <c r="AJ22">
+        <v>38</v>
+      </c>
+      <c r="AK22">
+        <v>15</v>
+      </c>
     </row>
-    <row r="23" spans="1:34" ht="64">
+    <row r="23" spans="1:37" ht="64">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5971,13 +6106,19 @@
         <v>53</v>
       </c>
       <c r="AG23" t="s">
-        <v>567</v>
-      </c>
-      <c r="AH23" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="AH23" t="s">
         <v>542</v>
       </c>
+      <c r="AJ23">
+        <v>37</v>
+      </c>
+      <c r="AK23">
+        <v>18</v>
+      </c>
     </row>
-    <row r="24" spans="1:34" ht="48">
+    <row r="24" spans="1:37" ht="48">
       <c r="A24">
         <v>23</v>
       </c>
@@ -6075,13 +6216,19 @@
         <v>107</v>
       </c>
       <c r="AG24" t="s">
-        <v>568</v>
-      </c>
-      <c r="AH24" s="12" t="s">
+        <v>567</v>
+      </c>
+      <c r="AH24" t="s">
         <v>543</v>
       </c>
+      <c r="AJ24">
+        <v>82</v>
+      </c>
+      <c r="AK24">
+        <v>81</v>
+      </c>
     </row>
-    <row r="25" spans="1:34" ht="48">
+    <row r="25" spans="1:37" ht="48">
       <c r="A25">
         <v>24</v>
       </c>
@@ -6179,13 +6326,19 @@
         <v>351</v>
       </c>
       <c r="AG25" t="s">
-        <v>569</v>
-      </c>
-      <c r="AH25" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="AH25" t="s">
         <v>544</v>
       </c>
+      <c r="AJ25">
+        <v>68</v>
+      </c>
+      <c r="AK25">
+        <v>83</v>
+      </c>
     </row>
-    <row r="26" spans="1:34" ht="80">
+    <row r="26" spans="1:37" ht="80">
       <c r="A26">
         <v>25</v>
       </c>
@@ -6283,10 +6436,16 @@
         <v>223</v>
       </c>
       <c r="AG26" t="s">
-        <v>570</v>
-      </c>
-      <c r="AH26" s="12" t="s">
+        <v>569</v>
+      </c>
+      <c r="AH26" t="s">
         <v>545</v>
+      </c>
+      <c r="AJ26">
+        <v>28</v>
+      </c>
+      <c r="AK26">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -6294,8 +6453,9 @@
   <hyperlinks>
     <hyperlink ref="AG2" r:id="rId1" xr:uid="{BDD1BE6A-FFCF-2246-A67F-9DD2A347B582}"/>
     <hyperlink ref="AH2" r:id="rId2" xr:uid="{78DD33E5-0BA4-0040-BED5-D7EDFA89F6A3}"/>
+    <hyperlink ref="AG11" r:id="rId3" xr:uid="{67F2C09B-7000-004D-8DF6-ADBCA7C962C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Feat] Setup DB from parsing xlsx file
</commit_message>
<xml_diff>
--- a/server/src/restinfos.xlsx
+++ b/server/src/restinfos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeomhyeji/Desktop/projects/MIJIworld/server/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1524D09-FB58-F244-BCAD-5144CFC15186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73A6E9A-F234-9845-8B47-ED0B28D742A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{21BFD20C-F461-4008-810F-8834C880AE86}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{21BFD20C-F461-4008-810F-8834C880AE86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="521">
   <si>
     <t>#0463D2</t>
   </si>
@@ -81,9 +81,6 @@
     <t>rest_kor</t>
   </si>
   <si>
-    <t>namemenu1</t>
-  </si>
-  <si>
     <t>namemenu2</t>
   </si>
   <si>
@@ -123,21 +120,6 @@
     <t>ratingnaver</t>
   </si>
   <si>
-    <t>ratinggoogle</t>
-  </si>
-  <si>
-    <t>raterskakao</t>
-  </si>
-  <si>
-    <t>ratersnaver</t>
-  </si>
-  <si>
-    <t>ratersgoogle</t>
-  </si>
-  <si>
-    <t>naverurl</t>
-  </si>
-  <si>
     <t>couscous</t>
   </si>
   <si>
@@ -365,24 +347,6 @@
   </si>
   <si>
     <t>세녹</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>apsara_angkor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>#F6E6FF</t>
-  </si>
-  <si>
-    <t>#032EA1</t>
-  </si>
-  <si>
-    <t>캄보디아</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>압사라 앙코르</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -876,9 +840,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>경기도 의정부시 태평로73번길 19</t>
-  </si>
-  <si>
     <t>매일 11:00 - 21:30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1290,30 +1251,6 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Leelawadee UI"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>ខ្ញុំនឹងរីករាយនឹងអាហារនេះ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>!</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
@@ -1849,14 +1786,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>압사라 앙코르는 현지인 셰프가 운영하는 캄보디아 음식 전문점입니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대체로 향신료가 강하지 않아 누구나 시도해보기 좋아요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>잘루스는 현지인 셰프가 운영하는 몽골 전문 음식점입니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1973,9 +1902,6 @@
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3165.9762748451417!2d126.97914721558675!3d37.48488623655712!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x357ca1b385d0fc03%3A0x591659184644e3f8!2sSENOK!5e0!3m2!1sko!2skr!4v1623562402338!5m2!1sko!2skr</t>
   </si>
   <si>
-    <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3155.1801438222196!2d127.04830951559195!3d37.73891782199405!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x357cc7685ba1801d%3A0x7944f2260e570a74!2z7JWV7IKs6528IOyVmey9lOultA!5e0!3m2!1sko!2skr!4v1623562430999!5m2!1sko!2skr</t>
-  </si>
-  <si>
     <t>https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3162.553654022189!2d127.00413831558865!3d37.565578531940105!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x357ca3229f39cd7b%3A0x80fe44907c8edfea!2z7J6Y66Oo7Iqk!5e0!3m2!1sko!2skr!4v1623562456631!5m2!1sko!2skr</t>
   </si>
   <si>
@@ -2076,10 +2002,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>기본 13,000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">사이드를 추가해 풍부하게 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2284,18 +2206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5,000/5,500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6,000/6,500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7,500/8,000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>진하고 향긋한</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2348,10 +2258,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8,000/12,000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>부드러운 닭고기가 올라간</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2468,50 +2374,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>록락</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>미차</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오리고기 볶음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캄보디아식 소고기 볶음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>얇은 소고기와 스모키한 소스를 넣은</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캄보디아식 볶음면</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에그 누들, 새우, 청경채가 들어간</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물씬 나는 오리고기 볶음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">매콤새콤 동남아시아 느낌이  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>양고기 볶음밥</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>개당 1,500</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>호쇼르</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2808,10 +2674,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>무한리필 이용시 무료</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이국적이고 진한 육향을 내는</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2908,73 +2770,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://map.naver.com/v5/entry/place/1351925028?c=14142945.2048704,4450344.2526898,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/30837121?c=14136084.4510694,4513735.9675140,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/1705124136?c=14130221.3536769,4510752.7102348,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/1873269440?c=14135948.0290334,4514596.7317776,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/32283786?c=14135948.0290334,4514596.7317776,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/1823834165?c=14135948.0290334,4514596.7317776,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/1790792517?c=14135948.0290334,4514596.7317776,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/37792177?c=14131122.7187258,4517241.4188359,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/31694764?c=14135948.0290334,4514596.7317776,15,0,0,0,dh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/460261321?c=14126475.1188532,4516439.1862914,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/19990202?c=14137758.3177247,4518178.8272255,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/36528615?c=14135032.5152773,4506911.2773203,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/585165741?c=14137822.0370012,4518247.4874901,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/36407019?c=14136924.4568150,4513631.3301334,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/11701020?c=14136924.4568150,4513631.3301334,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/11585347?c=14127509.7889923,4515800.7693440,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/141102773?c=14135931.5982766,4513778.2354726,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/21048818?c=14128063.5144034,4515810.8083695,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/13152789?c=14130892.3319076,4517325.0845137,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/12919183?c=14139079.0455593,4511549.3703520,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/20870613?c=14135965.7510964,4513798.3096542,15,0,0,0,dh</t>
-  </si>
-  <si>
-    <t>https://map.naver.com/v5/entry/place/35387377?c=14135127.4930668,4517223.2759138,15,0,0,0,dh</t>
-  </si>
-  <si>
     <t>https://place.map.kakao.com/14608358</t>
   </si>
   <si>
@@ -3017,9 +2812,6 @@
     <t>https://place.map.kakao.com/523907573</t>
   </si>
   <si>
-    <t>https://map.naver.com/v5/entry/place/245978217?c=14135991.5772182,4517324.1576999,19,0,0,0,dh</t>
-  </si>
-  <si>
     <t>https://place.map.kakao.com/21130631</t>
   </si>
   <si>
@@ -3047,9 +2839,6 @@
     <t>https://place.map.kakao.com/25462155</t>
   </si>
   <si>
-    <t>https://map.naver.com/v5/entry/place/1735679364?c=14143167.4097060,4542617.0198217,19,0,0,0,dh</t>
-  </si>
-  <si>
     <t>https://place.map.kakao.com/23642006</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3058,10 +2847,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://map.naver.com/v5/entry/place/34907751?c=14133888.3846828,4519968.3825312,15,0,0,0,dh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pintop</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3071,6 +2856,10 @@
   </si>
   <si>
     <t>https://place.map.kakao.com/1675286779</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>namemenu1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3078,7 +2867,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3153,14 +2942,6 @@
       <name val="Arial"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF404040"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3266,11 +3047,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3286,28 +3067,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3625,15 +3400,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41FF5E1-E7C0-4FE7-B208-B8C1E78BE041}">
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC9" zoomScale="131" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="131" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3677,19 +3452,19 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
+        <v>520</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
         <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
       </c>
       <c r="T1" t="s">
         <v>20</v>
@@ -3701,125 +3476,110 @@
         <v>22</v>
       </c>
       <c r="W1" t="s">
+        <v>16</v>
+      </c>
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
-        <v>28</v>
-      </c>
       <c r="AC1" t="s">
-        <v>29</v>
+        <v>516</v>
       </c>
       <c r="AD1" t="s">
-        <v>30</v>
+        <v>517</v>
       </c>
       <c r="AE1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>572</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>574</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>575</v>
+        <v>518</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:31">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="I2" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="K2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" t="s">
+      <c r="L2" t="s">
+        <v>260</v>
+      </c>
+      <c r="M2" t="s">
+        <v>213</v>
+      </c>
+      <c r="N2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>189</v>
-      </c>
-      <c r="J2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" t="s">
-        <v>275</v>
-      </c>
-      <c r="M2" t="s">
-        <v>226</v>
-      </c>
-      <c r="N2" t="s">
-        <v>43</v>
-      </c>
       <c r="O2" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="P2" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="Q2" t="s">
-        <v>299</v>
-      </c>
-      <c r="R2" t="s">
-        <v>305</v>
+        <v>290</v>
+      </c>
+      <c r="R2" s="9">
+        <v>19000</v>
       </c>
       <c r="S2" t="s">
-        <v>306</v>
-      </c>
-      <c r="T2" s="10">
-        <v>19000</v>
+        <v>285</v>
+      </c>
+      <c r="T2" t="s">
+        <v>286</v>
       </c>
       <c r="U2" t="s">
-        <v>302</v>
-      </c>
-      <c r="V2" t="s">
-        <v>303</v>
-      </c>
-      <c r="W2" s="10">
+        <v>287</v>
+      </c>
+      <c r="V2" s="9">
         <v>8000</v>
       </c>
+      <c r="W2" t="s">
+        <v>283</v>
+      </c>
       <c r="X2" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="Y2" t="s">
-        <v>300</v>
-      </c>
-      <c r="Z2" s="10">
+        <v>284</v>
+      </c>
+      <c r="Z2" s="9">
         <v>18000</v>
       </c>
       <c r="AA2">
@@ -3828,109 +3588,94 @@
       <c r="AB2">
         <v>4.37</v>
       </c>
-      <c r="AC2">
-        <v>3.9</v>
+      <c r="AC2" s="10" t="s">
+        <v>515</v>
       </c>
       <c r="AD2">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="AE2">
-        <v>22</v>
-      </c>
-      <c r="AF2">
-        <v>67</v>
-      </c>
-      <c r="AG2" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>573</v>
-      </c>
-      <c r="AJ2">
-        <v>45</v>
-      </c>
-      <c r="AK2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:31">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>178</v>
+      </c>
+      <c r="J3" t="s">
+        <v>214</v>
+      </c>
+      <c r="K3" t="s">
+        <v>215</v>
+      </c>
+      <c r="L3" t="s">
+        <v>291</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" t="s">
-        <v>190</v>
-      </c>
-      <c r="J3" t="s">
-        <v>227</v>
-      </c>
-      <c r="K3" t="s">
-        <v>228</v>
-      </c>
-      <c r="L3" t="s">
-        <v>307</v>
-      </c>
-      <c r="M3" t="s">
-        <v>49</v>
-      </c>
-      <c r="N3" t="s">
-        <v>50</v>
-      </c>
       <c r="O3" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="P3" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="Q3" t="s">
-        <v>311</v>
-      </c>
-      <c r="R3" t="s">
-        <v>312</v>
+        <v>297</v>
+      </c>
+      <c r="R3" s="9">
+        <v>18000</v>
       </c>
       <c r="S3" t="s">
-        <v>313</v>
-      </c>
-      <c r="T3" s="10">
-        <v>18000</v>
+        <v>294</v>
+      </c>
+      <c r="T3" t="s">
+        <v>298</v>
       </c>
       <c r="U3" t="s">
-        <v>314</v>
-      </c>
-      <c r="V3" t="s">
-        <v>315</v>
-      </c>
-      <c r="W3" s="10">
+        <v>299</v>
+      </c>
+      <c r="V3" s="9">
         <v>24000</v>
       </c>
+      <c r="W3" t="s">
+        <v>295</v>
+      </c>
       <c r="X3" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="Y3" t="s">
-        <v>318</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>316</v>
+        <v>301</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>13000</v>
       </c>
       <c r="AA3">
         <v>4</v>
@@ -3938,108 +3683,93 @@
       <c r="AB3">
         <v>4.5199999999999996</v>
       </c>
-      <c r="AC3">
-        <v>4.5</v>
+      <c r="AC3" t="s">
+        <v>492</v>
       </c>
       <c r="AD3">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="AE3">
-        <v>178</v>
-      </c>
-      <c r="AF3">
-        <v>912</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>546</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>525</v>
-      </c>
-      <c r="AJ3">
-        <v>82</v>
-      </c>
-      <c r="AK3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="48">
+    <row r="4" spans="1:31" ht="48">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="J4" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="K4" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="L4" t="s">
-        <v>276</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>213</v>
+        <v>261</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="P4" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="Q4" t="s">
-        <v>321</v>
-      </c>
-      <c r="R4" t="s">
-        <v>323</v>
+        <v>305</v>
+      </c>
+      <c r="R4" s="9">
+        <v>7900</v>
       </c>
       <c r="S4" t="s">
-        <v>322</v>
-      </c>
-      <c r="T4" s="10">
-        <v>7900</v>
+        <v>303</v>
+      </c>
+      <c r="T4" t="s">
+        <v>307</v>
       </c>
       <c r="U4" t="s">
-        <v>324</v>
-      </c>
-      <c r="V4" t="s">
-        <v>325</v>
-      </c>
-      <c r="W4" s="10">
+        <v>308</v>
+      </c>
+      <c r="V4" s="9">
         <v>10900</v>
       </c>
+      <c r="W4" t="s">
+        <v>304</v>
+      </c>
       <c r="X4" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="Y4" t="s">
-        <v>327</v>
-      </c>
-      <c r="Z4" s="10">
+        <v>310</v>
+      </c>
+      <c r="Z4" s="9">
         <v>13900</v>
       </c>
       <c r="AA4">
@@ -4048,102 +3778,93 @@
       <c r="AB4">
         <v>4.7</v>
       </c>
+      <c r="AC4" t="s">
+        <v>493</v>
+      </c>
       <c r="AD4">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="AE4">
-        <v>1</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>547</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>524</v>
-      </c>
-      <c r="AJ4">
-        <v>60</v>
-      </c>
-      <c r="AK4">
         <v>14.5</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="32">
+    <row r="5" spans="1:31" ht="32">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="I5" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="J5" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="K5" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="L5" t="s">
-        <v>277</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>217</v>
+        <v>262</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>205</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="O5" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="P5" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="Q5" t="s">
-        <v>330</v>
-      </c>
-      <c r="R5" t="s">
-        <v>331</v>
+        <v>315</v>
+      </c>
+      <c r="R5" s="9">
+        <v>12000</v>
       </c>
       <c r="S5" t="s">
-        <v>332</v>
-      </c>
-      <c r="T5" s="10">
-        <v>12000</v>
+        <v>312</v>
+      </c>
+      <c r="T5" t="s">
+        <v>316</v>
       </c>
       <c r="U5" t="s">
-        <v>333</v>
-      </c>
-      <c r="V5" t="s">
-        <v>334</v>
-      </c>
-      <c r="W5" s="10">
+        <v>317</v>
+      </c>
+      <c r="V5" s="9">
         <v>13000</v>
       </c>
+      <c r="W5" t="s">
+        <v>313</v>
+      </c>
       <c r="X5" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="Y5" t="s">
-        <v>336</v>
-      </c>
-      <c r="Z5" s="10">
+        <v>319</v>
+      </c>
+      <c r="Z5" s="9">
         <v>14000</v>
       </c>
       <c r="AA5">
@@ -4152,108 +3873,93 @@
       <c r="AB5">
         <v>4.7300000000000004</v>
       </c>
-      <c r="AC5">
-        <v>4.5</v>
+      <c r="AC5" t="s">
+        <v>494</v>
       </c>
       <c r="AD5">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="AE5">
-        <v>3</v>
-      </c>
-      <c r="AF5">
-        <v>6</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>548</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>526</v>
-      </c>
-      <c r="AJ5">
-        <v>59</v>
-      </c>
-      <c r="AK5">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="48">
+    <row r="6" spans="1:31" ht="48">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="J6" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="K6" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="L6" t="s">
-        <v>278</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>213</v>
+        <v>263</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="N6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="O6" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="P6" t="s">
-        <v>340</v>
+        <v>321</v>
       </c>
       <c r="Q6" t="s">
-        <v>343</v>
-      </c>
-      <c r="R6" t="s">
-        <v>338</v>
+        <v>322</v>
+      </c>
+      <c r="R6" s="9">
+        <v>13000</v>
       </c>
       <c r="S6" t="s">
-        <v>339</v>
-      </c>
-      <c r="T6" s="10">
-        <v>13000</v>
+        <v>323</v>
+      </c>
+      <c r="T6" t="s">
+        <v>324</v>
       </c>
       <c r="U6" t="s">
-        <v>341</v>
-      </c>
-      <c r="V6" t="s">
-        <v>342</v>
-      </c>
-      <c r="W6" s="10">
+        <v>325</v>
+      </c>
+      <c r="V6" s="9">
         <v>15000</v>
       </c>
+      <c r="W6" t="s">
+        <v>326</v>
+      </c>
       <c r="X6" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="Y6" t="s">
-        <v>345</v>
-      </c>
-      <c r="Z6" s="10">
+        <v>328</v>
+      </c>
+      <c r="Z6" s="9">
         <v>13000</v>
       </c>
       <c r="AA6">
@@ -4262,108 +3968,93 @@
       <c r="AB6">
         <v>4.1500000000000004</v>
       </c>
-      <c r="AC6">
-        <v>4</v>
+      <c r="AC6" t="s">
+        <v>495</v>
       </c>
       <c r="AD6">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="AE6">
-        <v>6</v>
-      </c>
-      <c r="AF6">
-        <v>48</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>549</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>527</v>
-      </c>
-      <c r="AJ6">
-        <v>56</v>
-      </c>
-      <c r="AK6">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:31">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="J7" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="K7" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="L7" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="M7" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="N7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="O7" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="P7" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="Q7" t="s">
-        <v>348</v>
-      </c>
-      <c r="R7" t="s">
-        <v>349</v>
+        <v>333</v>
+      </c>
+      <c r="R7" s="9">
+        <v>8000</v>
       </c>
       <c r="S7" t="s">
-        <v>350</v>
-      </c>
-      <c r="T7" s="10">
-        <v>8000</v>
+        <v>330</v>
+      </c>
+      <c r="T7" t="s">
+        <v>334</v>
       </c>
       <c r="U7" t="s">
-        <v>351</v>
-      </c>
-      <c r="V7" t="s">
-        <v>352</v>
-      </c>
-      <c r="W7" s="10">
+        <v>335</v>
+      </c>
+      <c r="V7" s="9">
         <v>12000</v>
       </c>
+      <c r="W7" t="s">
+        <v>331</v>
+      </c>
       <c r="X7" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="Y7" t="s">
-        <v>350</v>
-      </c>
-      <c r="Z7" s="10">
+        <v>333</v>
+      </c>
+      <c r="Z7" s="9">
         <v>8000</v>
       </c>
       <c r="AA7">
@@ -4372,108 +4063,93 @@
       <c r="AB7">
         <v>4.58</v>
       </c>
-      <c r="AC7">
-        <v>4.5</v>
+      <c r="AC7" t="s">
+        <v>496</v>
       </c>
       <c r="AD7">
-        <v>113</v>
+        <v>47</v>
       </c>
       <c r="AE7">
-        <v>313</v>
-      </c>
-      <c r="AF7">
-        <v>435</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>550</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>528</v>
-      </c>
-      <c r="AJ7">
-        <v>47</v>
-      </c>
-      <c r="AK7">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:31">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="I8" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="J8" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="K8" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="L8" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="M8" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="N8" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="O8" t="s">
-        <v>354</v>
+        <v>337</v>
       </c>
       <c r="P8" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="Q8" t="s">
-        <v>356</v>
-      </c>
-      <c r="R8" t="s">
-        <v>359</v>
+        <v>343</v>
+      </c>
+      <c r="R8" s="9">
+        <v>10000</v>
       </c>
       <c r="S8" t="s">
-        <v>360</v>
-      </c>
-      <c r="T8" s="10">
-        <v>10000</v>
+        <v>338</v>
+      </c>
+      <c r="T8" t="s">
+        <v>340</v>
       </c>
       <c r="U8" t="s">
-        <v>357</v>
-      </c>
-      <c r="V8" t="s">
-        <v>358</v>
-      </c>
-      <c r="W8" s="10">
+        <v>341</v>
+      </c>
+      <c r="V8" s="9">
         <v>3000</v>
       </c>
+      <c r="W8" t="s">
+        <v>339</v>
+      </c>
       <c r="X8" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="Y8" t="s">
-        <v>362</v>
-      </c>
-      <c r="Z8" s="10">
+        <v>345</v>
+      </c>
+      <c r="Z8" s="9">
         <v>8000</v>
       </c>
       <c r="AA8">
@@ -4482,109 +4158,94 @@
       <c r="AB8">
         <v>2.86</v>
       </c>
-      <c r="AC8">
-        <v>4.3</v>
+      <c r="AC8" t="s">
+        <v>497</v>
       </c>
       <c r="AD8">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="AE8">
-        <v>3</v>
-      </c>
-      <c r="AF8">
-        <v>36</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>551</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>529</v>
-      </c>
-      <c r="AJ8">
-        <v>51</v>
-      </c>
-      <c r="AK8">
         <v>21.5</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="48">
+    <row r="9" spans="1:31" ht="48">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="J9" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="K9" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="L9" t="s">
-        <v>281</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>213</v>
+        <v>266</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="N9" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="O9" t="s">
-        <v>363</v>
+        <v>346</v>
       </c>
       <c r="P9" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="Q9" t="s">
-        <v>365</v>
-      </c>
-      <c r="R9" t="s">
-        <v>366</v>
+        <v>350</v>
+      </c>
+      <c r="R9">
+        <v>5500</v>
       </c>
       <c r="S9" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
       <c r="T9" t="s">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="U9" t="s">
-        <v>371</v>
-      </c>
-      <c r="V9" t="s">
-        <v>372</v>
+        <v>352</v>
+      </c>
+      <c r="V9">
+        <v>6500</v>
       </c>
       <c r="W9" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="X9" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
       <c r="Y9" t="s">
-        <v>374</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>370</v>
+        <v>354</v>
+      </c>
+      <c r="Z9">
+        <v>8000</v>
       </c>
       <c r="AA9">
         <v>4.0999999999999996</v>
@@ -4592,108 +4253,93 @@
       <c r="AB9">
         <v>4.26</v>
       </c>
-      <c r="AC9">
-        <v>4.3</v>
+      <c r="AC9" t="s">
+        <v>498</v>
       </c>
       <c r="AD9">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="AE9">
-        <v>105</v>
-      </c>
-      <c r="AF9">
-        <v>196</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>552</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>530</v>
-      </c>
-      <c r="AJ9">
-        <v>66</v>
-      </c>
-      <c r="AK9">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="48">
+    <row r="10" spans="1:31" ht="48">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="I10" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="J10" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="K10" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="L10" t="s">
-        <v>282</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>213</v>
+        <v>267</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="N10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="O10" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="P10" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="Q10" t="s">
-        <v>376</v>
-      </c>
-      <c r="R10" t="s">
-        <v>377</v>
+        <v>358</v>
+      </c>
+      <c r="R10" s="9">
+        <v>11000</v>
       </c>
       <c r="S10" t="s">
-        <v>378</v>
-      </c>
-      <c r="T10" s="10">
-        <v>11000</v>
+        <v>355</v>
+      </c>
+      <c r="T10" t="s">
+        <v>359</v>
       </c>
       <c r="U10" t="s">
-        <v>379</v>
-      </c>
-      <c r="V10" t="s">
-        <v>380</v>
-      </c>
-      <c r="W10" s="10">
+        <v>360</v>
+      </c>
+      <c r="V10" s="9">
         <v>10000</v>
       </c>
+      <c r="W10" t="s">
+        <v>356</v>
+      </c>
       <c r="X10" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="Y10" t="s">
-        <v>382</v>
-      </c>
-      <c r="Z10" s="10">
+        <v>362</v>
+      </c>
+      <c r="Z10" s="9">
         <v>15000</v>
       </c>
       <c r="AA10">
@@ -4702,85 +4348,70 @@
       <c r="AB10">
         <v>4.7</v>
       </c>
-      <c r="AC10">
-        <v>4.0999999999999996</v>
+      <c r="AC10" t="s">
+        <v>499</v>
       </c>
       <c r="AD10">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="AE10">
-        <v>2</v>
-      </c>
-      <c r="AF10">
-        <v>12</v>
-      </c>
-      <c r="AG10" t="s">
-        <v>553</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>532</v>
-      </c>
-      <c r="AJ10">
-        <v>61</v>
-      </c>
-      <c r="AK10">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:31">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" t="s">
+        <v>185</v>
+      </c>
+      <c r="J11" t="s">
+        <v>232</v>
+      </c>
+      <c r="K11" t="s">
+        <v>233</v>
+      </c>
+      <c r="L11" t="s">
+        <v>268</v>
+      </c>
+      <c r="M11" t="s">
+        <v>206</v>
+      </c>
+      <c r="N11" t="s">
         <v>83</v>
       </c>
-      <c r="C11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>87</v>
-      </c>
-      <c r="G11" t="s">
-        <v>88</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I11" t="s">
-        <v>197</v>
-      </c>
-      <c r="J11" t="s">
-        <v>245</v>
-      </c>
-      <c r="K11" t="s">
-        <v>246</v>
-      </c>
-      <c r="L11" t="s">
-        <v>283</v>
-      </c>
-      <c r="M11" t="s">
-        <v>218</v>
-      </c>
-      <c r="N11" t="s">
-        <v>89</v>
-      </c>
       <c r="O11" t="s">
-        <v>383</v>
-      </c>
-      <c r="R11" t="s">
-        <v>385</v>
-      </c>
-      <c r="S11" t="s">
-        <v>386</v>
-      </c>
-      <c r="T11" t="s">
-        <v>384</v>
+        <v>363</v>
+      </c>
+      <c r="P11" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>365</v>
+      </c>
+      <c r="R11">
+        <v>12000</v>
       </c>
       <c r="AA11">
         <v>4.5</v>
@@ -4788,108 +4419,93 @@
       <c r="AB11">
         <v>4.57</v>
       </c>
-      <c r="AC11">
-        <v>4.4000000000000004</v>
+      <c r="AC11" s="10" t="s">
+        <v>519</v>
       </c>
       <c r="AD11">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="AE11">
-        <v>92</v>
-      </c>
-      <c r="AF11">
-        <v>102</v>
-      </c>
-      <c r="AG11" s="11" t="s">
-        <v>576</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>531</v>
-      </c>
-      <c r="AJ11">
-        <v>66</v>
-      </c>
-      <c r="AK11">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:31">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
         <v>85</v>
       </c>
-      <c r="E12" t="s">
-        <v>91</v>
-      </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="I12" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="J12" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="K12" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="L12" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="M12" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="N12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="P12" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="Q12" t="s">
-        <v>389</v>
-      </c>
-      <c r="R12" t="s">
-        <v>395</v>
+        <v>373</v>
+      </c>
+      <c r="R12" s="9">
+        <v>12000</v>
       </c>
       <c r="S12" t="s">
-        <v>394</v>
-      </c>
-      <c r="T12" s="10">
-        <v>12000</v>
+        <v>367</v>
+      </c>
+      <c r="T12" t="s">
+        <v>371</v>
       </c>
       <c r="U12" t="s">
-        <v>392</v>
-      </c>
-      <c r="V12" t="s">
-        <v>393</v>
-      </c>
-      <c r="W12" s="10">
+        <v>372</v>
+      </c>
+      <c r="V12" s="9">
         <v>9500</v>
       </c>
+      <c r="W12" t="s">
+        <v>368</v>
+      </c>
       <c r="X12" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="Y12" t="s">
-        <v>391</v>
-      </c>
-      <c r="Z12" s="10">
+        <v>370</v>
+      </c>
+      <c r="Z12" s="9">
         <v>8000</v>
       </c>
       <c r="AA12">
@@ -4898,108 +4514,93 @@
       <c r="AB12">
         <v>4.5599999999999996</v>
       </c>
-      <c r="AC12">
-        <v>4.5</v>
+      <c r="AC12" t="s">
+        <v>500</v>
       </c>
       <c r="AD12">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="AE12">
-        <v>334</v>
-      </c>
-      <c r="AF12">
-        <v>187</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>554</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>533</v>
-      </c>
-      <c r="AJ12">
-        <v>55</v>
-      </c>
-      <c r="AK12">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:31">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I13" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="J13" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="K13" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="L13" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="M13" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="N13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="O13" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="P13" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
       <c r="Q13" t="s">
-        <v>397</v>
-      </c>
-      <c r="R13" t="s">
-        <v>399</v>
+        <v>379</v>
+      </c>
+      <c r="R13" s="9">
+        <v>10000</v>
       </c>
       <c r="S13" t="s">
-        <v>400</v>
-      </c>
-      <c r="T13" s="10">
-        <v>10000</v>
+        <v>377</v>
+      </c>
+      <c r="T13" t="s">
+        <v>380</v>
       </c>
       <c r="U13" t="s">
-        <v>401</v>
-      </c>
-      <c r="V13" t="s">
-        <v>402</v>
-      </c>
-      <c r="W13" s="10">
+        <v>381</v>
+      </c>
+      <c r="V13" s="9">
         <v>7000</v>
       </c>
+      <c r="W13" t="s">
+        <v>376</v>
+      </c>
       <c r="X13" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="Y13" t="s">
-        <v>404</v>
-      </c>
-      <c r="Z13" s="10">
+        <v>383</v>
+      </c>
+      <c r="Z13" s="9">
         <v>7000</v>
       </c>
       <c r="AA13">
@@ -5008,108 +4609,93 @@
       <c r="AB13">
         <v>4.3899999999999997</v>
       </c>
-      <c r="AC13">
-        <v>4</v>
+      <c r="AC13" t="s">
+        <v>501</v>
       </c>
       <c r="AD13">
-        <v>113</v>
+        <v>38</v>
       </c>
       <c r="AE13">
-        <v>117</v>
-      </c>
-      <c r="AF13">
-        <v>542</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>555</v>
-      </c>
-      <c r="AH13" t="s">
-        <v>534</v>
-      </c>
-      <c r="AJ13">
-        <v>38</v>
-      </c>
-      <c r="AK13">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:31">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="I14" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="J14" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="K14" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="L14" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="M14" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="N14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="O14" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="P14" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
       <c r="Q14" t="s">
-        <v>407</v>
-      </c>
-      <c r="R14" t="s">
-        <v>408</v>
+        <v>388</v>
+      </c>
+      <c r="R14" s="9">
+        <v>7500</v>
       </c>
       <c r="S14" t="s">
-        <v>409</v>
-      </c>
-      <c r="T14" s="10">
-        <v>7500</v>
+        <v>385</v>
+      </c>
+      <c r="T14" t="s">
+        <v>389</v>
       </c>
       <c r="U14" t="s">
-        <v>410</v>
-      </c>
-      <c r="V14" t="s">
-        <v>411</v>
-      </c>
-      <c r="W14" s="10">
+        <v>390</v>
+      </c>
+      <c r="V14" s="9">
         <v>8000</v>
       </c>
+      <c r="W14" t="s">
+        <v>386</v>
+      </c>
       <c r="X14" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="Y14" t="s">
-        <v>413</v>
-      </c>
-      <c r="Z14" s="10">
+        <v>392</v>
+      </c>
+      <c r="Z14" s="9">
         <v>8500</v>
       </c>
       <c r="AA14">
@@ -5118,534 +4704,471 @@
       <c r="AB14">
         <v>4.2300000000000004</v>
       </c>
-      <c r="AC14">
-        <v>3.7</v>
+      <c r="AC14" t="s">
+        <v>502</v>
       </c>
       <c r="AD14">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="AE14">
-        <v>677</v>
-      </c>
-      <c r="AF14">
-        <v>492</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>556</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>535</v>
-      </c>
-      <c r="AJ14">
-        <v>61</v>
-      </c>
-      <c r="AK14">
         <v>34.5</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="18">
+    <row r="15" spans="1:31">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" t="s">
+        <v>187</v>
+      </c>
+      <c r="J15" t="s">
+        <v>240</v>
+      </c>
+      <c r="K15" t="s">
+        <v>241</v>
+      </c>
+      <c r="L15" t="s">
+        <v>272</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="N15" t="s">
+        <v>104</v>
+      </c>
+      <c r="O15" t="s">
+        <v>395</v>
+      </c>
+      <c r="P15" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>399</v>
+      </c>
+      <c r="R15" s="9">
+        <v>8000</v>
+      </c>
+      <c r="S15" t="s">
+        <v>393</v>
+      </c>
+      <c r="T15" t="s">
+        <v>400</v>
+      </c>
+      <c r="U15" t="s">
+        <v>401</v>
+      </c>
+      <c r="V15" s="9">
+        <v>7000</v>
+      </c>
+      <c r="W15" t="s">
+        <v>394</v>
+      </c>
+      <c r="X15" t="s">
+        <v>397</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>1500</v>
+      </c>
+      <c r="AA15">
+        <v>4.2</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>503</v>
+      </c>
+      <c r="AD15">
+        <v>59</v>
+      </c>
+      <c r="AE15">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
         <v>106</v>
       </c>
-      <c r="C15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F16" t="s">
         <v>107</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G16" t="s">
         <v>108</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="I16" t="s">
+        <v>189</v>
+      </c>
+      <c r="J16" t="s">
+        <v>242</v>
+      </c>
+      <c r="K16" t="s">
+        <v>243</v>
+      </c>
+      <c r="L16" t="s">
+        <v>273</v>
+      </c>
+      <c r="M16" t="s">
+        <v>211</v>
+      </c>
+      <c r="N16" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="J15" t="s">
-        <v>253</v>
-      </c>
-      <c r="K15" t="s">
-        <v>254</v>
-      </c>
-      <c r="L15" t="s">
-        <v>287</v>
-      </c>
-      <c r="M15" t="s">
-        <v>222</v>
-      </c>
-      <c r="N15" t="s">
-        <v>110</v>
-      </c>
-      <c r="O15" t="s">
-        <v>414</v>
-      </c>
-      <c r="P15" t="s">
-        <v>415</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>416</v>
-      </c>
-      <c r="R15" t="s">
-        <v>418</v>
-      </c>
-      <c r="S15" t="s">
-        <v>417</v>
-      </c>
-      <c r="T15" s="10">
-        <v>8000</v>
-      </c>
-      <c r="U15" t="s">
-        <v>420</v>
-      </c>
-      <c r="V15" t="s">
-        <v>419</v>
-      </c>
-      <c r="W15" s="10">
-        <v>8000</v>
-      </c>
-      <c r="X15" t="s">
-        <v>422</v>
-      </c>
-      <c r="Y15" t="s">
-        <v>421</v>
-      </c>
-      <c r="Z15" s="10">
-        <v>12000</v>
-      </c>
-      <c r="AA15">
-        <v>5</v>
-      </c>
-      <c r="AD15">
-        <v>1</v>
-      </c>
-      <c r="AG15" t="s">
-        <v>557</v>
-      </c>
-      <c r="AH15" t="s">
-        <v>570</v>
-      </c>
-      <c r="AJ15">
-        <v>59</v>
-      </c>
-      <c r="AK15">
-        <v>40.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>111</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" t="s">
-        <v>114</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I16" t="s">
-        <v>199</v>
-      </c>
-      <c r="J16" t="s">
-        <v>255</v>
-      </c>
-      <c r="K16" t="s">
-        <v>256</v>
-      </c>
-      <c r="L16" t="s">
-        <v>288</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="N16" t="s">
-        <v>115</v>
-      </c>
       <c r="O16" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
       <c r="P16" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="Q16" t="s">
-        <v>425</v>
-      </c>
-      <c r="R16" t="s">
-        <v>429</v>
+        <v>405</v>
+      </c>
+      <c r="R16" s="9">
+        <v>7500</v>
       </c>
       <c r="S16" t="s">
-        <v>430</v>
-      </c>
-      <c r="T16" s="10">
-        <v>8000</v>
+        <v>403</v>
+      </c>
+      <c r="T16" t="s">
+        <v>408</v>
       </c>
       <c r="U16" t="s">
-        <v>431</v>
-      </c>
-      <c r="V16" t="s">
-        <v>432</v>
-      </c>
-      <c r="W16" s="10">
+        <v>407</v>
+      </c>
+      <c r="V16" s="9">
         <v>7000</v>
       </c>
+      <c r="W16" t="s">
+        <v>404</v>
+      </c>
       <c r="X16" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
       <c r="Y16" t="s">
-        <v>427</v>
-      </c>
-      <c r="Z16" s="10" t="s">
-        <v>424</v>
+        <v>410</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>3000</v>
       </c>
       <c r="AA16">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="AB16">
         <v>4.33</v>
       </c>
-      <c r="AC16">
-        <v>4.3</v>
+      <c r="AC16" t="s">
+        <v>504</v>
       </c>
       <c r="AD16">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="AE16">
-        <v>48</v>
-      </c>
-      <c r="AF16">
-        <v>289</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>558</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>536</v>
-      </c>
-      <c r="AJ16">
-        <v>37</v>
-      </c>
-      <c r="AK16">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:31">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F17" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>186</v>
+        <v>113</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="I17" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="J17" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="K17" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="L17" t="s">
-        <v>289</v>
-      </c>
-      <c r="M17" t="s">
-        <v>224</v>
+        <v>274</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="N17" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="O17" t="s">
-        <v>433</v>
+        <v>411</v>
       </c>
       <c r="P17" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="Q17" t="s">
-        <v>435</v>
-      </c>
-      <c r="R17" t="s">
-        <v>437</v>
+        <v>393</v>
+      </c>
+      <c r="R17" s="9">
+        <v>12000</v>
       </c>
       <c r="S17" t="s">
-        <v>436</v>
-      </c>
-      <c r="T17" s="10">
-        <v>7500</v>
+        <v>412</v>
+      </c>
+      <c r="T17" t="s">
+        <v>415</v>
       </c>
       <c r="U17" t="s">
-        <v>439</v>
-      </c>
-      <c r="V17" t="s">
-        <v>438</v>
-      </c>
-      <c r="W17" s="10">
-        <v>7000</v>
+        <v>416</v>
+      </c>
+      <c r="V17" s="9">
+        <v>14000</v>
+      </c>
+      <c r="W17" t="s">
+        <v>413</v>
       </c>
       <c r="X17" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="Y17" t="s">
-        <v>441</v>
-      </c>
-      <c r="Z17" s="10">
-        <v>3000</v>
+        <v>418</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>13000</v>
       </c>
       <c r="AA17">
-        <v>3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AB17">
         <v>4.54</v>
       </c>
-      <c r="AC17">
-        <v>4.4000000000000004</v>
+      <c r="AC17" t="s">
+        <v>505</v>
       </c>
       <c r="AD17">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="AE17">
-        <v>71</v>
-      </c>
-      <c r="AF17">
-        <v>995</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>559</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>560</v>
-      </c>
-      <c r="AJ17">
-        <v>65</v>
-      </c>
-      <c r="AK17">
         <v>42.5</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:31">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E18" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F18" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="G18" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="I18" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="J18" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="K18" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="L18" t="s">
-        <v>290</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>225</v>
+        <v>275</v>
+      </c>
+      <c r="M18" t="s">
+        <v>213</v>
       </c>
       <c r="N18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="O18" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="P18" t="s">
-        <v>443</v>
+        <v>424</v>
       </c>
       <c r="Q18" t="s">
-        <v>444</v>
-      </c>
-      <c r="R18" t="s">
-        <v>445</v>
+        <v>425</v>
+      </c>
+      <c r="R18" s="9">
+        <v>26000</v>
       </c>
       <c r="S18" t="s">
+        <v>420</v>
+      </c>
+      <c r="T18" t="s">
+        <v>422</v>
+      </c>
+      <c r="U18" t="s">
         <v>423</v>
       </c>
-      <c r="T18" s="10">
+      <c r="V18" s="9">
+        <v>8000</v>
+      </c>
+      <c r="W18" t="s">
+        <v>421</v>
+      </c>
+      <c r="X18" t="s">
+        <v>427</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>426</v>
+      </c>
+      <c r="Z18" s="9">
         <v>12000</v>
       </c>
-      <c r="U18" t="s">
-        <v>446</v>
-      </c>
-      <c r="V18" t="s">
-        <v>447</v>
-      </c>
-      <c r="W18" s="10">
-        <v>14000</v>
-      </c>
-      <c r="X18" t="s">
-        <v>448</v>
-      </c>
-      <c r="Y18" t="s">
-        <v>449</v>
-      </c>
-      <c r="Z18" s="10">
-        <v>13000</v>
-      </c>
       <c r="AA18">
-        <v>4.0999999999999996</v>
+        <v>3.7</v>
       </c>
       <c r="AB18">
         <v>5</v>
       </c>
-      <c r="AC18">
-        <v>4.5</v>
+      <c r="AC18" t="s">
+        <v>506</v>
       </c>
       <c r="AD18">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="AE18">
-        <v>1</v>
-      </c>
-      <c r="AF18">
-        <v>53</v>
-      </c>
-      <c r="AG18" t="s">
-        <v>561</v>
-      </c>
-      <c r="AH18" t="s">
-        <v>537</v>
-      </c>
-      <c r="AJ18">
-        <v>49</v>
-      </c>
-      <c r="AK18">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:31" ht="42">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="I19" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="J19" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="K19" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="L19" t="s">
-        <v>291</v>
-      </c>
-      <c r="M19" t="s">
-        <v>226</v>
+        <v>276</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="N19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="O19" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="P19" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="Q19" t="s">
-        <v>452</v>
-      </c>
-      <c r="R19" t="s">
-        <v>455</v>
+        <v>433</v>
+      </c>
+      <c r="R19" s="9">
+        <v>13000</v>
       </c>
       <c r="S19" t="s">
-        <v>456</v>
-      </c>
-      <c r="T19" s="10">
-        <v>26000</v>
+        <v>430</v>
+      </c>
+      <c r="T19" t="s">
+        <v>436</v>
       </c>
       <c r="U19" t="s">
-        <v>453</v>
-      </c>
-      <c r="V19" t="s">
-        <v>454</v>
-      </c>
-      <c r="W19" s="10">
-        <v>8000</v>
+        <v>435</v>
+      </c>
+      <c r="V19" s="9">
+        <v>16000</v>
+      </c>
+      <c r="W19" t="s">
+        <v>428</v>
       </c>
       <c r="X19" t="s">
-        <v>458</v>
+        <v>431</v>
       </c>
       <c r="Y19" t="s">
-        <v>457</v>
-      </c>
-      <c r="Z19" s="10">
-        <v>12000</v>
+        <v>432</v>
+      </c>
+      <c r="Z19" s="9">
+        <v>14000</v>
       </c>
       <c r="AA19">
         <v>3.7</v>
@@ -5653,809 +5176,607 @@
       <c r="AB19">
         <v>4.5599999999999996</v>
       </c>
-      <c r="AC19">
-        <v>4.5</v>
+      <c r="AC19" t="s">
+        <v>507</v>
       </c>
       <c r="AD19">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="AE19">
-        <v>147</v>
-      </c>
-      <c r="AF19">
-        <v>1116</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>562</v>
-      </c>
-      <c r="AH19" t="s">
-        <v>538</v>
-      </c>
-      <c r="AJ19">
-        <v>48</v>
-      </c>
-      <c r="AK19">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="64">
+    <row r="20" spans="1:31" ht="48">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G20" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="I20" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="J20" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="K20" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="L20" t="s">
-        <v>292</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>216</v>
+        <v>277</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="N20" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="O20" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="P20" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="Q20" t="s">
-        <v>459</v>
-      </c>
-      <c r="R20" t="s">
-        <v>465</v>
+        <v>441</v>
+      </c>
+      <c r="R20" s="9">
+        <v>16000</v>
       </c>
       <c r="S20" t="s">
-        <v>464</v>
-      </c>
-      <c r="T20" s="10">
-        <v>13000</v>
+        <v>438</v>
+      </c>
+      <c r="T20" t="s">
+        <v>442</v>
       </c>
       <c r="U20" t="s">
-        <v>467</v>
-      </c>
-      <c r="V20" t="s">
-        <v>466</v>
-      </c>
-      <c r="W20" s="10">
-        <v>16000</v>
+        <v>443</v>
+      </c>
+      <c r="V20" s="9">
+        <v>31000</v>
+      </c>
+      <c r="W20" t="s">
+        <v>439</v>
       </c>
       <c r="X20" t="s">
-        <v>462</v>
+        <v>444</v>
       </c>
       <c r="Y20" t="s">
-        <v>463</v>
-      </c>
-      <c r="Z20" s="10">
-        <v>14000</v>
+        <v>445</v>
+      </c>
+      <c r="Z20" s="9">
+        <v>60000</v>
       </c>
       <c r="AA20">
-        <v>3.7</v>
+        <v>4.2</v>
       </c>
       <c r="AB20">
         <v>4.54</v>
       </c>
-      <c r="AC20">
-        <v>4.0999999999999996</v>
+      <c r="AC20" t="s">
+        <v>508</v>
       </c>
       <c r="AD20">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AE20">
-        <v>56</v>
-      </c>
-      <c r="AF20">
-        <v>136</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>563</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>539</v>
-      </c>
-      <c r="AJ20">
-        <v>43</v>
-      </c>
-      <c r="AK20">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="48">
+    <row r="21" spans="1:31" ht="32">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" t="s">
         <v>132</v>
       </c>
-      <c r="D21" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" t="s">
-        <v>138</v>
-      </c>
       <c r="F21" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="G21" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I21" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="J21" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="K21" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="L21" t="s">
-        <v>293</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>213</v>
+        <v>278</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="N21" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="O21" t="s">
-        <v>468</v>
+        <v>446</v>
       </c>
       <c r="P21" t="s">
-        <v>469</v>
+        <v>451</v>
       </c>
       <c r="Q21" t="s">
-        <v>470</v>
-      </c>
-      <c r="R21" t="s">
-        <v>471</v>
+        <v>452</v>
+      </c>
+      <c r="R21" s="9">
+        <v>9100</v>
       </c>
       <c r="S21" t="s">
-        <v>472</v>
-      </c>
-      <c r="T21" s="10">
-        <v>16000</v>
+        <v>447</v>
+      </c>
+      <c r="T21" t="s">
+        <v>453</v>
       </c>
       <c r="U21" t="s">
-        <v>473</v>
-      </c>
-      <c r="V21" t="s">
-        <v>474</v>
-      </c>
-      <c r="W21" s="10">
-        <v>31000</v>
+        <v>454</v>
+      </c>
+      <c r="V21" s="9">
+        <v>8800</v>
+      </c>
+      <c r="W21" t="s">
+        <v>448</v>
       </c>
       <c r="X21" t="s">
-        <v>475</v>
+        <v>450</v>
       </c>
       <c r="Y21" t="s">
-        <v>476</v>
-      </c>
-      <c r="Z21" s="10">
-        <v>60000</v>
+        <v>449</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>7900</v>
       </c>
       <c r="AA21">
-        <v>4.2</v>
+        <v>3.7</v>
       </c>
       <c r="AB21">
         <v>4.43</v>
       </c>
-      <c r="AC21">
+      <c r="AC21" t="s">
+        <v>509</v>
+      </c>
+      <c r="AD21">
+        <v>43</v>
+      </c>
+      <c r="AE21">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="64">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" t="s">
+        <v>139</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I22" t="s">
+        <v>194</v>
+      </c>
+      <c r="J22" t="s">
+        <v>254</v>
+      </c>
+      <c r="K22" t="s">
+        <v>457</v>
+      </c>
+      <c r="L22" t="s">
+        <v>279</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="N22" t="s">
+        <v>140</v>
+      </c>
+      <c r="O22" t="s">
+        <v>455</v>
+      </c>
+      <c r="P22" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>462</v>
+      </c>
+      <c r="R22" s="9">
+        <v>5000</v>
+      </c>
+      <c r="S22" t="s">
+        <v>456</v>
+      </c>
+      <c r="T22" t="s">
+        <v>458</v>
+      </c>
+      <c r="U22" t="s">
+        <v>459</v>
+      </c>
+      <c r="V22" s="9">
+        <v>3000</v>
+      </c>
+      <c r="W22" t="s">
+        <v>460</v>
+      </c>
+      <c r="X22" t="s">
+        <v>463</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>464</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>5000</v>
+      </c>
+      <c r="AA22">
         <v>4.5999999999999996</v>
-      </c>
-      <c r="AD21">
-        <v>32</v>
-      </c>
-      <c r="AE21">
-        <v>161</v>
-      </c>
-      <c r="AF21">
-        <v>454</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>564</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>540</v>
-      </c>
-      <c r="AJ21">
-        <v>43</v>
-      </c>
-      <c r="AK21">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:37" ht="32">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>142</v>
-      </c>
-      <c r="C22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G22" t="s">
-        <v>145</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="I22" t="s">
-        <v>205</v>
-      </c>
-      <c r="J22" t="s">
-        <v>267</v>
-      </c>
-      <c r="K22" t="s">
-        <v>268</v>
-      </c>
-      <c r="L22" t="s">
-        <v>294</v>
-      </c>
-      <c r="M22" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="N22" t="s">
-        <v>146</v>
-      </c>
-      <c r="O22" t="s">
-        <v>477</v>
-      </c>
-      <c r="P22" t="s">
-        <v>478</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>479</v>
-      </c>
-      <c r="R22" t="s">
-        <v>482</v>
-      </c>
-      <c r="S22" t="s">
-        <v>483</v>
-      </c>
-      <c r="T22" s="10">
-        <v>9100</v>
-      </c>
-      <c r="U22" t="s">
-        <v>484</v>
-      </c>
-      <c r="V22" t="s">
-        <v>485</v>
-      </c>
-      <c r="W22" s="10">
-        <v>8800</v>
-      </c>
-      <c r="X22" t="s">
-        <v>481</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>480</v>
-      </c>
-      <c r="Z22" s="10">
-        <v>7900</v>
-      </c>
-      <c r="AA22">
-        <v>3.7</v>
       </c>
       <c r="AB22">
         <v>4.49</v>
       </c>
-      <c r="AC22">
-        <v>4.3</v>
+      <c r="AC22" t="s">
+        <v>510</v>
       </c>
       <c r="AD22">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="AE22">
-        <v>248</v>
-      </c>
-      <c r="AF22">
-        <v>164</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>565</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>541</v>
-      </c>
-      <c r="AJ22">
-        <v>38</v>
-      </c>
-      <c r="AK22">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="64">
+    <row r="23" spans="1:31" ht="48">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G23" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="I23" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="J23" t="s">
-        <v>269</v>
+        <v>480</v>
       </c>
       <c r="K23" t="s">
-        <v>488</v>
+        <v>255</v>
       </c>
       <c r="L23" t="s">
-        <v>295</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>214</v>
+        <v>280</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="N23" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="O23" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="P23" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="Q23" t="s">
-        <v>491</v>
-      </c>
-      <c r="R23" t="s">
-        <v>492</v>
+        <v>477</v>
+      </c>
+      <c r="R23" s="9">
+        <v>40000</v>
       </c>
       <c r="S23" t="s">
-        <v>493</v>
-      </c>
-      <c r="T23" s="10">
-        <v>5000</v>
+        <v>479</v>
+      </c>
+      <c r="T23" t="s">
+        <v>482</v>
       </c>
       <c r="U23" t="s">
-        <v>489</v>
-      </c>
-      <c r="V23" t="s">
-        <v>490</v>
-      </c>
-      <c r="W23" s="10">
-        <v>3000</v>
+        <v>481</v>
+      </c>
+      <c r="V23" s="9">
+        <v>6000</v>
+      </c>
+      <c r="W23" t="s">
+        <v>473</v>
       </c>
       <c r="X23" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="Y23" t="s">
-        <v>495</v>
-      </c>
-      <c r="Z23" s="10">
-        <v>5000</v>
+        <v>474</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>18000</v>
       </c>
       <c r="AA23">
-        <v>4.5999999999999996</v>
+        <v>4</v>
       </c>
       <c r="AB23">
         <v>4.6500000000000004</v>
       </c>
-      <c r="AC23">
-        <v>4.4000000000000004</v>
+      <c r="AC23" t="s">
+        <v>511</v>
       </c>
       <c r="AD23">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="AE23">
-        <v>457</v>
-      </c>
-      <c r="AF23">
-        <v>53</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>566</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>542</v>
-      </c>
-      <c r="AJ23">
-        <v>37</v>
-      </c>
-      <c r="AK23">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="48">
+    <row r="24" spans="1:31" ht="48">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F24" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="G24" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="I24" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="J24" t="s">
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="K24" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="L24" t="s">
-        <v>296</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>215</v>
+        <v>281</v>
+      </c>
+      <c r="M24" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="N24" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="O24" t="s">
-        <v>508</v>
+        <v>469</v>
       </c>
       <c r="P24" t="s">
-        <v>511</v>
+        <v>468</v>
       </c>
       <c r="Q24" t="s">
-        <v>505</v>
-      </c>
-      <c r="R24" t="s">
-        <v>510</v>
+        <v>471</v>
+      </c>
+      <c r="R24" s="9">
+        <v>29000</v>
       </c>
       <c r="S24" t="s">
-        <v>509</v>
-      </c>
-      <c r="T24" s="10">
-        <v>40000</v>
+        <v>470</v>
+      </c>
+      <c r="T24" t="s">
+        <v>472</v>
       </c>
       <c r="U24" t="s">
-        <v>514</v>
-      </c>
-      <c r="V24" t="s">
-        <v>513</v>
-      </c>
-      <c r="W24" s="10">
-        <v>6000</v>
+        <v>471</v>
+      </c>
+      <c r="V24" s="9">
+        <v>35000</v>
+      </c>
+      <c r="W24" t="s">
+        <v>465</v>
       </c>
       <c r="X24" t="s">
-        <v>507</v>
+        <v>466</v>
       </c>
       <c r="Y24" t="s">
-        <v>506</v>
-      </c>
-      <c r="Z24" s="10">
-        <v>18000</v>
+        <v>467</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
       </c>
       <c r="AA24">
-        <v>4</v>
+        <v>3.8</v>
       </c>
       <c r="AB24">
         <v>4.75</v>
       </c>
-      <c r="AC24">
-        <v>4.3</v>
+      <c r="AC24" t="s">
+        <v>512</v>
       </c>
       <c r="AD24">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="AE24">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="80">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
         <v>151</v>
       </c>
-      <c r="AF24">
-        <v>107</v>
-      </c>
-      <c r="AG24" t="s">
-        <v>567</v>
-      </c>
-      <c r="AH24" t="s">
-        <v>543</v>
-      </c>
-      <c r="AJ24">
-        <v>82</v>
-      </c>
-      <c r="AK24">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:37" ht="48">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>157</v>
-      </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F25" t="s">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>160</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>184</v>
+        <v>153</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="I25" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="J25" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="K25" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="L25" t="s">
-        <v>297</v>
-      </c>
-      <c r="M25" s="6" t="s">
-        <v>210</v>
+        <v>282</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="N25" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="O25" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="P25" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="Q25" t="s">
-        <v>496</v>
-      </c>
-      <c r="R25" t="s">
-        <v>500</v>
+        <v>487</v>
+      </c>
+      <c r="R25" s="9">
+        <v>16000</v>
       </c>
       <c r="S25" t="s">
-        <v>503</v>
-      </c>
-      <c r="T25" s="10">
-        <v>29000</v>
+        <v>483</v>
+      </c>
+      <c r="T25" t="s">
+        <v>485</v>
       </c>
       <c r="U25" t="s">
-        <v>504</v>
-      </c>
-      <c r="V25" t="s">
-        <v>503</v>
-      </c>
-      <c r="W25" s="10">
-        <v>35000</v>
+        <v>484</v>
+      </c>
+      <c r="V25" s="9">
+        <v>17000</v>
+      </c>
+      <c r="W25" t="s">
+        <v>489</v>
       </c>
       <c r="X25" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="Y25" t="s">
-        <v>498</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>499</v>
+        <v>490</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>19000</v>
       </c>
       <c r="AA25">
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="AB25">
         <v>4.46</v>
       </c>
-      <c r="AC25">
-        <v>4.2</v>
+      <c r="AC25" t="s">
+        <v>513</v>
       </c>
       <c r="AD25">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="AE25">
-        <v>35</v>
-      </c>
-      <c r="AF25">
-        <v>351</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>568</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>544</v>
-      </c>
-      <c r="AJ25">
-        <v>68</v>
-      </c>
-      <c r="AK25">
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="80">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>162</v>
-      </c>
-      <c r="C26" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" t="s">
-        <v>163</v>
-      </c>
-      <c r="F26" t="s">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
-        <v>164</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="I26" t="s">
-        <v>209</v>
-      </c>
-      <c r="J26" t="s">
-        <v>273</v>
-      </c>
-      <c r="K26" t="s">
-        <v>274</v>
-      </c>
-      <c r="L26" t="s">
-        <v>298</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="N26" t="s">
-        <v>165</v>
-      </c>
-      <c r="O26" t="s">
-        <v>518</v>
-      </c>
-      <c r="P26" t="s">
-        <v>515</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>521</v>
-      </c>
-      <c r="R26" t="s">
-        <v>520</v>
-      </c>
-      <c r="S26" t="s">
-        <v>519</v>
-      </c>
-      <c r="T26" s="10">
-        <v>16000</v>
-      </c>
-      <c r="U26" t="s">
-        <v>517</v>
-      </c>
-      <c r="V26" t="s">
-        <v>516</v>
-      </c>
-      <c r="W26" s="10">
-        <v>17000</v>
-      </c>
-      <c r="X26" t="s">
-        <v>523</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>522</v>
-      </c>
-      <c r="Z26" s="10">
-        <v>19000</v>
-      </c>
-      <c r="AA26">
-        <v>4.5</v>
-      </c>
+    <row r="26" spans="1:31">
       <c r="AB26">
         <v>5</v>
       </c>
-      <c r="AC26">
-        <v>4.5</v>
+      <c r="AC26" t="s">
+        <v>514</v>
       </c>
       <c r="AD26">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="AE26">
-        <v>3</v>
-      </c>
-      <c r="AF26">
-        <v>223</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>569</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>545</v>
-      </c>
-      <c r="AJ26">
-        <v>28</v>
-      </c>
-      <c r="AK26">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="AG2" r:id="rId1" xr:uid="{BDD1BE6A-FFCF-2246-A67F-9DD2A347B582}"/>
-    <hyperlink ref="AH2" r:id="rId2" xr:uid="{78DD33E5-0BA4-0040-BED5-D7EDFA89F6A3}"/>
-    <hyperlink ref="AG11" r:id="rId3" xr:uid="{67F2C09B-7000-004D-8DF6-ADBCA7C962C5}"/>
+    <hyperlink ref="AC2" r:id="rId1" xr:uid="{BDD1BE6A-FFCF-2246-A67F-9DD2A347B582}"/>
+    <hyperlink ref="AC11" r:id="rId2" xr:uid="{67F2C09B-7000-004D-8DF6-ADBCA7C962C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Feat] Setup DB from scraping
</commit_message>
<xml_diff>
--- a/server/src/restinfos.xlsx
+++ b/server/src/restinfos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeomhyeji/Desktop/projects/MIJIworld/server/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73A6E9A-F234-9845-8B47-ED0B28D742A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC859B79-D72E-1E49-BB28-C3E02F039C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{21BFD20C-F461-4008-810F-8834C880AE86}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="543">
   <si>
     <t>#0463D2</t>
   </si>
@@ -2836,9 +2836,6 @@
     <t>https://place.map.kakao.com/17357597</t>
   </si>
   <si>
-    <t>https://place.map.kakao.com/25462155</t>
-  </si>
-  <si>
     <t>https://place.map.kakao.com/23642006</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2861,6 +2858,76 @@
   <si>
     <t>namemenu1</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>naverPlaceUrl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5GywN2l6</t>
+  </si>
+  <si>
+    <t>https://naver.me/5On93MHs</t>
+  </si>
+  <si>
+    <t>https://naver.me/x9LgiJ2R</t>
+  </si>
+  <si>
+    <t>https://naver.me/GNy6CHfW</t>
+  </si>
+  <si>
+    <t>https://naver.me/xmrHAKBa</t>
+  </si>
+  <si>
+    <t>https://naver.me/5L3dgXyA</t>
+  </si>
+  <si>
+    <t>https://naver.me/GQ4OFWHF</t>
+  </si>
+  <si>
+    <t>https://naver.me/xaPuSkys</t>
+  </si>
+  <si>
+    <t>https://naver.me/5X9p62AZ</t>
+  </si>
+  <si>
+    <t>https://naver.me/GkKhCpEv</t>
+  </si>
+  <si>
+    <t>https://naver.me/5zJkKdG4</t>
+  </si>
+  <si>
+    <t>https://naver.me/FCbsFDHb</t>
+  </si>
+  <si>
+    <t>https://naver.me/5DHgpYCH</t>
+  </si>
+  <si>
+    <t>https://naver.me/GEAnmV7k</t>
+  </si>
+  <si>
+    <t>https://naver.me/FlJwqsOD</t>
+  </si>
+  <si>
+    <t>https://naver.me/FKKG0F00</t>
+  </si>
+  <si>
+    <t>https://naver.me/GcjKdEIz</t>
+  </si>
+  <si>
+    <t>https://naver.me/xrPzfxWi</t>
+  </si>
+  <si>
+    <t>https://naver.me/5AmSDHn6</t>
+  </si>
+  <si>
+    <t>https://naver.me/59jXODvJ</t>
+  </si>
+  <si>
+    <t>https://naver.me/FPsngYjo</t>
+  </si>
+  <si>
+    <t>https://naver.me/I5FvnEVf</t>
   </si>
 </sst>
 </file>
@@ -3400,15 +3467,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F41FF5E1-E7C0-4FE7-B208-B8C1E78BE041}">
-  <dimension ref="A1:AE26"/>
+  <dimension ref="A1:AF25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="131" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="V20" zoomScale="131" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3452,7 +3519,7 @@
         <v>14</v>
       </c>
       <c r="O1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="P1" t="s">
         <v>17</v>
@@ -3494,16 +3561,19 @@
         <v>27</v>
       </c>
       <c r="AC1" t="s">
+        <v>515</v>
+      </c>
+      <c r="AD1" t="s">
         <v>516</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>517</v>
       </c>
-      <c r="AE1" t="s">
-        <v>518</v>
+      <c r="AF1" t="s">
+        <v>520</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
+    <row r="2" spans="1:32">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3589,7 +3659,7 @@
         <v>4.37</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AD2">
         <v>45</v>
@@ -3597,8 +3667,11 @@
       <c r="AE2">
         <v>17</v>
       </c>
+      <c r="AF2" s="10" t="s">
+        <v>521</v>
+      </c>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:32">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3692,8 +3765,11 @@
       <c r="AE3">
         <v>20</v>
       </c>
+      <c r="AF3" s="10" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="4" spans="1:31" ht="48">
+    <row r="4" spans="1:32" ht="48">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3787,8 +3863,11 @@
       <c r="AE4">
         <v>14.5</v>
       </c>
+      <c r="AF4" s="10" t="s">
+        <v>523</v>
+      </c>
     </row>
-    <row r="5" spans="1:31" ht="32">
+    <row r="5" spans="1:32" ht="32">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3882,8 +3961,9 @@
       <c r="AE5">
         <v>25</v>
       </c>
+      <c r="AF5" s="10"/>
     </row>
-    <row r="6" spans="1:31" ht="48">
+    <row r="6" spans="1:32" ht="48">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3977,8 +4057,11 @@
       <c r="AE6">
         <v>11</v>
       </c>
+      <c r="AF6" t="s">
+        <v>524</v>
+      </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:32">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4072,8 +4155,11 @@
       <c r="AE7">
         <v>13</v>
       </c>
+      <c r="AF7" s="10" t="s">
+        <v>525</v>
+      </c>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:32">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4167,8 +4253,11 @@
       <c r="AE8">
         <v>21.5</v>
       </c>
+      <c r="AF8" s="10" t="s">
+        <v>526</v>
+      </c>
     </row>
-    <row r="9" spans="1:31" ht="48">
+    <row r="9" spans="1:32" ht="48">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4262,8 +4351,11 @@
       <c r="AE9">
         <v>24</v>
       </c>
+      <c r="AF9" s="10" t="s">
+        <v>527</v>
+      </c>
     </row>
-    <row r="10" spans="1:31" ht="48">
+    <row r="10" spans="1:32" ht="48">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4357,8 +4449,11 @@
       <c r="AE10">
         <v>17</v>
       </c>
+      <c r="AF10" s="10" t="s">
+        <v>528</v>
+      </c>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:32">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4420,7 +4515,7 @@
         <v>4.57</v>
       </c>
       <c r="AC11" s="10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AD11">
         <v>66</v>
@@ -4428,8 +4523,11 @@
       <c r="AE11">
         <v>44</v>
       </c>
+      <c r="AF11" s="10" t="s">
+        <v>529</v>
+      </c>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:32">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4523,8 +4621,11 @@
       <c r="AE12">
         <v>40</v>
       </c>
+      <c r="AF12" s="10" t="s">
+        <v>530</v>
+      </c>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:32">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4618,8 +4719,11 @@
       <c r="AE13">
         <v>30</v>
       </c>
+      <c r="AF13" s="10" t="s">
+        <v>531</v>
+      </c>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:32">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4713,8 +4817,11 @@
       <c r="AE14">
         <v>34.5</v>
       </c>
+      <c r="AF14" s="10" t="s">
+        <v>533</v>
+      </c>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:32">
       <c r="A15">
         <v>15</v>
       </c>
@@ -4805,8 +4912,11 @@
       <c r="AE15">
         <v>40.5</v>
       </c>
+      <c r="AF15" s="10" t="s">
+        <v>532</v>
+      </c>
     </row>
-    <row r="16" spans="1:31">
+    <row r="16" spans="1:32">
       <c r="A16">
         <v>16</v>
       </c>
@@ -4900,8 +5010,11 @@
       <c r="AE16">
         <v>39</v>
       </c>
+      <c r="AF16" s="10" t="s">
+        <v>534</v>
+      </c>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:32">
       <c r="A17">
         <v>17</v>
       </c>
@@ -4995,8 +5108,11 @@
       <c r="AE17">
         <v>42.5</v>
       </c>
+      <c r="AF17" s="10" t="s">
+        <v>535</v>
+      </c>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:32">
       <c r="A18">
         <v>18</v>
       </c>
@@ -5090,8 +5206,11 @@
       <c r="AE18">
         <v>31</v>
       </c>
+      <c r="AF18" s="10" t="s">
+        <v>536</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" ht="42">
+    <row r="19" spans="1:32" ht="42">
       <c r="A19">
         <v>19</v>
       </c>
@@ -5185,8 +5304,11 @@
       <c r="AE19">
         <v>24</v>
       </c>
+      <c r="AF19" s="10" t="s">
+        <v>537</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" ht="48">
+    <row r="20" spans="1:32" ht="48">
       <c r="A20">
         <v>20</v>
       </c>
@@ -5280,8 +5402,11 @@
       <c r="AE20">
         <v>20</v>
       </c>
+      <c r="AF20" s="10" t="s">
+        <v>538</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" ht="32">
+    <row r="21" spans="1:32" ht="32">
       <c r="A21">
         <v>21</v>
       </c>
@@ -5375,8 +5500,11 @@
       <c r="AE21">
         <v>72</v>
       </c>
+      <c r="AF21" s="10" t="s">
+        <v>539</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" ht="64">
+    <row r="22" spans="1:32" ht="64">
       <c r="A22">
         <v>22</v>
       </c>
@@ -5470,8 +5598,11 @@
       <c r="AE22">
         <v>15</v>
       </c>
+      <c r="AF22" s="10" t="s">
+        <v>540</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" ht="48">
+    <row r="23" spans="1:32" ht="48">
       <c r="A23">
         <v>23</v>
       </c>
@@ -5566,7 +5697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="48">
+    <row r="24" spans="1:32" ht="48">
       <c r="A24">
         <v>24</v>
       </c>
@@ -5660,8 +5791,11 @@
       <c r="AE24">
         <v>81</v>
       </c>
+      <c r="AF24" s="10" t="s">
+        <v>541</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" ht="80">
+    <row r="25" spans="1:32" ht="80">
       <c r="A25">
         <v>25</v>
       </c>
@@ -5755,19 +5889,8 @@
       <c r="AE25">
         <v>83</v>
       </c>
-    </row>
-    <row r="26" spans="1:31">
-      <c r="AB26">
-        <v>5</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>514</v>
-      </c>
-      <c r="AD26">
-        <v>28</v>
-      </c>
-      <c r="AE26">
-        <v>18</v>
+      <c r="AF25" s="10" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -5775,8 +5898,29 @@
   <hyperlinks>
     <hyperlink ref="AC2" r:id="rId1" xr:uid="{BDD1BE6A-FFCF-2246-A67F-9DD2A347B582}"/>
     <hyperlink ref="AC11" r:id="rId2" xr:uid="{67F2C09B-7000-004D-8DF6-ADBCA7C962C5}"/>
+    <hyperlink ref="AF2" r:id="rId3" xr:uid="{1354923E-71D4-274B-942C-D0DF5086EB8F}"/>
+    <hyperlink ref="AF3" r:id="rId4" xr:uid="{535AE102-56E5-BB4F-AA51-99C3E3695089}"/>
+    <hyperlink ref="AF4" r:id="rId5" xr:uid="{B58CEE95-07D6-DB48-A351-DA45DB557506}"/>
+    <hyperlink ref="AF7" r:id="rId6" xr:uid="{D5738C09-7D2D-7043-8246-6FDD952A4B6C}"/>
+    <hyperlink ref="AF8" r:id="rId7" xr:uid="{9C0BCFC6-DBE4-2D4D-AAEB-ADECA2C6F3CE}"/>
+    <hyperlink ref="AF9" r:id="rId8" xr:uid="{2F8C80E3-23D5-7B47-A9DB-6EF7E3CE22E5}"/>
+    <hyperlink ref="AF10" r:id="rId9" xr:uid="{56BABBB8-6AFF-1647-AE13-295AB64EADF1}"/>
+    <hyperlink ref="AF11" r:id="rId10" xr:uid="{714B18D2-9CF8-CD47-A55B-839749BE469F}"/>
+    <hyperlink ref="AF12" r:id="rId11" xr:uid="{05F217D6-FD8C-204B-9966-917C2D49467E}"/>
+    <hyperlink ref="AF13" r:id="rId12" xr:uid="{4373D87D-75A6-8340-B2FC-5DFE8AD582CF}"/>
+    <hyperlink ref="AF15" r:id="rId13" xr:uid="{F0C04634-220B-7149-8013-3381AB1F8D94}"/>
+    <hyperlink ref="AF14" r:id="rId14" xr:uid="{21CD64E8-2427-7F4D-9F6E-68C79B5DAADD}"/>
+    <hyperlink ref="AF16" r:id="rId15" xr:uid="{A051CB20-14B3-F343-BE63-BBBC02B06610}"/>
+    <hyperlink ref="AF17" r:id="rId16" xr:uid="{AE3D0AE7-C6C9-2D45-A1D4-254078203B53}"/>
+    <hyperlink ref="AF18" r:id="rId17" xr:uid="{F8BB3AA2-0813-F34B-AFE1-F2263CAF2108}"/>
+    <hyperlink ref="AF19" r:id="rId18" xr:uid="{BD0E4F46-A930-3342-B809-93D452990C29}"/>
+    <hyperlink ref="AF20" r:id="rId19" xr:uid="{91AA46C5-6725-014E-86B0-D9C9512F2DA6}"/>
+    <hyperlink ref="AF21" r:id="rId20" xr:uid="{9DD51BB9-89C8-1C46-A2AE-F3076C63C71C}"/>
+    <hyperlink ref="AF22" r:id="rId21" xr:uid="{222217BD-15B4-1A4E-B38F-1AD77D9B7965}"/>
+    <hyperlink ref="AF24" r:id="rId22" xr:uid="{05A91D24-75C1-874F-B4D0-A60115CF6811}"/>
+    <hyperlink ref="AF25" r:id="rId23" xr:uid="{19214369-2480-3645-B085-60D07F562473}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>